<commit_message>
Dehydration validation table tweak.
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/Scenarios/DehydrationManual.xlsx
+++ b/data/human/adult/validation/Scenarios/DehydrationManual.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse\dehydration\source\data\human\adult\validation\Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A0EEC37-5B39-4A74-A59E-296A1E45BEE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F26BA2B1-2B8E-4AE6-B7B0-919C72197276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14940" yWindow="10170" windowWidth="31815" windowHeight="19155" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="9105" windowWidth="33195" windowHeight="19155" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Manual" sheetId="10" r:id="rId1"/>
@@ -104,15 +104,6 @@
     <t>Yellow</t>
   </si>
   <si>
-    <t>&gt;1% lost (by weight) @cite gellert2015signs</t>
-  </si>
-  <si>
-    <t>&gt;2% (by weight) lost @cite gellert2015signs</t>
-  </si>
-  <si>
-    <t>&gt;5% lost (by weight) @cite gellert2015signs</t>
-  </si>
-  <si>
     <t>TotalFluidVolume(L)</t>
   </si>
   <si>
@@ -258,6 +249,15 @@
   </si>
   <si>
     <t>|&lt;span class="warning"&gt;</t>
+  </si>
+  <si>
+    <t>&gt;3% lost (by weight) @cite gellert2015signs</t>
+  </si>
+  <si>
+    <t>&gt;5% (by weight) lost @cite gellert2015signs</t>
+  </si>
+  <si>
+    <t>&gt;10% lost (by weight) @cite gellert2015signs</t>
   </si>
 </sst>
 </file>
@@ -777,7 +777,7 @@
   <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -913,7 +913,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>0</v>
@@ -931,19 +931,19 @@
         <v>3</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>26</v>
+        <v>75</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>27</v>
+        <v>76</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>2</v>
@@ -955,7 +955,7 @@
         <v>3</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="Q3" s="2" t="s">
         <v>2</v>
@@ -966,13 +966,13 @@
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>0</v>
@@ -1002,7 +1002,7 @@
         <v>2</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="O4" s="2" t="s">
         <v>3</v>
@@ -1019,37 +1019,37 @@
         <v>0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="K5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>2</v>
@@ -1072,7 +1072,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>0</v>
@@ -1090,19 +1090,19 @@
         <v>0</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>2</v>
@@ -1114,7 +1114,7 @@
         <v>3</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="Q6" s="2" t="s">
         <v>2</v>
@@ -1125,49 +1125,49 @@
         <v>0</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="P7" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="P7" s="4" t="s">
-        <v>44</v>
       </c>
       <c r="Q7" s="2" t="s">
         <v>2</v>
@@ -1178,7 +1178,7 @@
         <v>0</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>0</v>
@@ -1193,7 +1193,7 @@
         <v>34.1</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H8" s="9" t="s">
         <v>13</v>
@@ -1202,10 +1202,10 @@
         <v>2</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L8" s="9" t="s">
         <v>13</v>
@@ -1214,7 +1214,7 @@
         <v>2</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="O8" s="2" t="s">
         <v>3</v>
@@ -1231,13 +1231,13 @@
         <v>0</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>0</v>
@@ -1249,25 +1249,25 @@
         <v>0</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>0</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M9" s="2" t="s">
         <v>0</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="O9" s="2" t="s">
         <v>3</v>
@@ -1284,13 +1284,13 @@
         <v>0</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>0</v>
@@ -1308,7 +1308,7 @@
         <v>2</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>3</v>
@@ -1320,7 +1320,7 @@
         <v>2</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="O10" s="2" t="s">
         <v>3</v>
@@ -1337,13 +1337,13 @@
         <v>0</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>0</v>
@@ -1361,7 +1361,7 @@
         <v>2</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>3</v>
@@ -1373,7 +1373,7 @@
         <v>2</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="O11" s="2" t="s">
         <v>3</v>
@@ -1390,13 +1390,13 @@
         <v>0</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>0</v>
@@ -1414,7 +1414,7 @@
         <v>2</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>3</v>
@@ -1426,7 +1426,7 @@
         <v>2</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="O12" s="2" t="s">
         <v>3</v>
@@ -1443,7 +1443,7 @@
         <v>0</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>0</v>
@@ -1496,7 +1496,7 @@
         <v>0</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>0</v>
@@ -1511,7 +1511,7 @@
         <v>4500</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H14" s="9" t="s">
         <v>14</v>
@@ -1523,7 +1523,7 @@
         <v>3430</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="L14" s="10" t="s">
         <v>14</v>
@@ -1535,7 +1535,7 @@
         <v>1990</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="P14" s="10" t="s">
         <v>16</v>
@@ -1549,7 +1549,7 @@
         <v>0</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>0</v>
@@ -1561,7 +1561,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>3</v>
@@ -1573,7 +1573,7 @@
         <v>2</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>3</v>
@@ -1585,7 +1585,7 @@
         <v>2</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="O15" s="2" t="s">
         <v>3</v>

</xml_diff>